<commit_message>
Enter Description for understanding the excel file
</commit_message>
<xml_diff>
--- a/AutonomousRacing_Literature.xlsx
+++ b/AutonomousRacing_Literature.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johannesbetz/Documents/03_UPenn/05_Paper/Autonomous_Racing_Review/literature/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johannesbetz/Documents/99_Programming/AutonomousRacing_Literature/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33CE86F-DA54-7443-91C0-966FA19C3258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5759E7-53B0-864C-9D73-785804F6C24B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26480" xr2:uid="{C9A78CC6-6B2A-6642-AAF0-EDC9630CD29D}"/>
+    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="26480" xr2:uid="{C9A78CC6-6B2A-6642-AAF0-EDC9630CD29D}"/>
   </bookViews>
   <sheets>
     <sheet name="Paper Overview" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
move stahl et al to evaluation category
</commit_message>
<xml_diff>
--- a/AutonomousRacing_Literature.xlsx
+++ b/AutonomousRacing_Literature.xlsx
@@ -951,6 +951,9 @@
     <t xml:space="preserve">https://ieeexplore-ieee-org.proxy.library.upenn.edu/document/9304722</t>
   </si>
   <si>
+    <t xml:space="preserve">1- Evaluation</t>
+  </si>
+  <si>
     <t xml:space="preserve">Online Verification Enabling Approval of Driving Functions—Implementation for a Planner of an Autonomous Race Vehicle</t>
   </si>
   <si>
@@ -1454,9 +1457,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://citeseerx.ist.psu.edu/viewdoc/download?doi=10.1.1.710.6672&amp;rep=rep1&amp;type=pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1- Evaluation</t>
   </si>
   <si>
     <t xml:space="preserve">Overall Racing Comparison</t>
@@ -2982,7 +2982,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3171,11 +3171,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="9815137"/>
-        <c:axId val="84369432"/>
+        <c:axId val="52899356"/>
+        <c:axId val="94820870"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="9815137"/>
+        <c:axId val="52899356"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2009"/>
@@ -3253,13 +3253,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84369432"/>
+        <c:crossAx val="94820870"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="84369432"/>
+        <c:axId val="94820870"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3336,7 +3336,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9815137"/>
+        <c:crossAx val="52899356"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3410,8 +3410,8 @@
   </sheetPr>
   <dimension ref="A1:P228"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A58" activeCellId="0" sqref="58:58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="65:65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6149,10 +6149,10 @@
         <v>67</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>142</v>
+        <v>250</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>280</v>
@@ -6176,10 +6176,10 @@
         <v>38</v>
       </c>
       <c r="L65" s="8" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6187,7 +6187,7 @@
         <v>2014</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>142</v>
@@ -6214,16 +6214,16 @@
         <v>88</v>
       </c>
       <c r="K66" s="12" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L66" s="8" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="M66" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6231,7 +6231,7 @@
         <v>2015</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>142</v>
@@ -6243,7 +6243,7 @@
         <v>144</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>21</v>
@@ -6258,16 +6258,16 @@
         <v>88</v>
       </c>
       <c r="K67" s="12" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L67" s="8" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="M67" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6275,7 +6275,7 @@
         <v>2018</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>142</v>
@@ -6299,16 +6299,16 @@
         <v>88</v>
       </c>
       <c r="K68" s="12" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L68" s="8" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="M68" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6316,7 +6316,7 @@
         <v>2020</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>142</v>
@@ -6340,16 +6340,16 @@
         <v>88</v>
       </c>
       <c r="K69" s="12" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L69" s="8" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="M69" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N69" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6357,7 +6357,7 @@
         <v>2016</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>142</v>
@@ -6369,7 +6369,7 @@
         <v>144</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="G70" s="8" t="s">
         <v>21</v>
@@ -6384,16 +6384,16 @@
         <v>88</v>
       </c>
       <c r="K70" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L70" s="8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M70" s="1" t="s">
         <v>162</v>
       </c>
       <c r="N70" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6401,7 +6401,7 @@
         <v>2017</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>142</v>
@@ -6413,7 +6413,7 @@
         <v>159</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>21</v>
@@ -6428,16 +6428,16 @@
         <v>88</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L71" s="8" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="M71" s="1" t="s">
         <v>162</v>
       </c>
       <c r="N71" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6445,7 +6445,7 @@
         <v>2018</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>142</v>
@@ -6454,10 +6454,10 @@
         <v>143</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G72" s="8" t="s">
         <v>21</v>
@@ -6472,16 +6472,16 @@
         <v>88</v>
       </c>
       <c r="K72" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L72" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="M72" s="1" t="s">
         <v>162</v>
       </c>
       <c r="N72" s="2" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6489,7 +6489,7 @@
         <v>2021</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>142</v>
@@ -6498,10 +6498,10 @@
         <v>143</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>21</v>
@@ -6516,16 +6516,16 @@
         <v>88</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L73" s="8" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="M73" s="1" t="s">
         <v>162</v>
       </c>
       <c r="N73" s="9" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6533,7 +6533,7 @@
         <v>2017</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>142</v>
@@ -6545,7 +6545,7 @@
         <v>159</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>21</v>
@@ -6560,14 +6560,14 @@
         <v>88</v>
       </c>
       <c r="K74" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L74" s="5" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="M74" s="5"/>
       <c r="N74" s="6" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O74" s="5"/>
       <c r="P74" s="5"/>
@@ -6577,7 +6577,7 @@
         <v>2020</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>142</v>
@@ -6586,7 +6586,7 @@
         <v>143</v>
       </c>
       <c r="E75" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>176</v>
@@ -6607,13 +6607,13 @@
         <v>89</v>
       </c>
       <c r="L75" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N75" s="9" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6621,7 +6621,7 @@
         <v>2020</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>142</v>
@@ -6630,7 +6630,7 @@
         <v>143</v>
       </c>
       <c r="E76" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F76" s="8" t="s">
         <v>155</v>
@@ -6651,10 +6651,10 @@
         <v>89</v>
       </c>
       <c r="L76" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6662,7 +6662,7 @@
         <v>2021</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>142</v>
@@ -6674,7 +6674,7 @@
         <v>144</v>
       </c>
       <c r="F77" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="G77" s="8" t="s">
         <v>21</v>
@@ -6692,10 +6692,10 @@
         <v>89</v>
       </c>
       <c r="L77" s="8" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="N77" s="6" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6703,7 +6703,7 @@
         <v>2021</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>142</v>
@@ -6715,7 +6715,7 @@
         <v>144</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="G78" s="8" t="s">
         <v>21</v>
@@ -6733,10 +6733,10 @@
         <v>89</v>
       </c>
       <c r="L78" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6744,7 +6744,7 @@
         <v>2021</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>142</v>
@@ -6753,10 +6753,10 @@
         <v>143</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="G79" s="8" t="s">
         <v>21</v>
@@ -6774,10 +6774,10 @@
         <v>89</v>
       </c>
       <c r="L79" s="8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="N79" s="6" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6785,7 +6785,7 @@
         <v>2019</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>142</v>
@@ -6812,16 +6812,16 @@
         <v>88</v>
       </c>
       <c r="K80" s="8" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="L80" s="8" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="M80" s="1" t="s">
         <v>234</v>
       </c>
       <c r="N80" s="2" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6829,7 +6829,7 @@
         <v>2021</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>142</v>
@@ -6856,16 +6856,16 @@
         <v>88</v>
       </c>
       <c r="K81" s="8" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="L81" s="8" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="M81" s="1" t="s">
         <v>234</v>
       </c>
       <c r="N81" s="6" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6873,7 +6873,7 @@
         <v>2020</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C82" s="8" t="s">
         <v>142</v>
@@ -6900,13 +6900,13 @@
         <v>88</v>
       </c>
       <c r="K82" s="8" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="L82" s="8" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="N82" s="9" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6942,13 +6942,13 @@
         <v>97</v>
       </c>
       <c r="L83" s="8" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="M83" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N83" s="2" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6956,7 +6956,7 @@
         <v>2021</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>142</v>
@@ -6986,13 +6986,13 @@
         <v>97</v>
       </c>
       <c r="L84" s="8" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="M84" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7000,7 +7000,7 @@
         <v>2020</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C85" s="8" t="s">
         <v>142</v>
@@ -7012,7 +7012,7 @@
         <v>144</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="G85" s="8" t="s">
         <v>21</v>
@@ -7030,10 +7030,10 @@
         <v>97</v>
       </c>
       <c r="L85" s="8" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="N85" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7041,19 +7041,19 @@
         <v>2021</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="G86" s="8" t="s">
         <v>21</v>
@@ -7071,13 +7071,13 @@
         <v>22</v>
       </c>
       <c r="L86" s="8" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="M86" s="1" t="s">
         <v>54</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7085,19 +7085,19 @@
         <v>2021</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="G87" s="1" t="s">
         <v>21</v>
@@ -7115,13 +7115,13 @@
         <v>22</v>
       </c>
       <c r="L87" s="8" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="M87" s="1" t="s">
         <v>54</v>
       </c>
       <c r="N87" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7129,19 +7129,19 @@
         <v>2020</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>21</v>
@@ -7159,13 +7159,13 @@
         <v>22</v>
       </c>
       <c r="L88" s="8" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="N88" s="6" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7173,19 +7173,19 @@
         <v>2020</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G89" s="8" t="s">
         <v>21</v>
@@ -7203,13 +7203,13 @@
         <v>22</v>
       </c>
       <c r="L89" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="M89" s="8" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="N89" s="11" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7217,19 +7217,19 @@
         <v>2017</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G90" s="1" t="s">
         <v>21</v>
@@ -7247,10 +7247,10 @@
         <v>22</v>
       </c>
       <c r="L90" s="8" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N90" s="6" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="91" s="5" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7258,19 +7258,19 @@
         <v>2018</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="G91" s="1" t="s">
         <v>21</v>
@@ -7288,11 +7288,11 @@
         <v>22</v>
       </c>
       <c r="L91" s="8" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="M91" s="1"/>
       <c r="N91" s="6" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="O91" s="1"/>
       <c r="P91" s="1"/>
@@ -7302,19 +7302,19 @@
         <v>2018</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>21</v>
@@ -7332,11 +7332,11 @@
         <v>22</v>
       </c>
       <c r="L92" s="8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="M92" s="1"/>
       <c r="N92" s="6" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="O92" s="1"/>
       <c r="P92" s="1"/>
@@ -7346,19 +7346,19 @@
         <v>2019</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>21</v>
@@ -7376,11 +7376,11 @@
         <v>22</v>
       </c>
       <c r="L93" s="8" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="M93" s="1"/>
       <c r="N93" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="O93" s="1"/>
       <c r="P93" s="1"/>
@@ -7390,19 +7390,19 @@
         <v>2019</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>21</v>
@@ -7420,11 +7420,11 @@
         <v>22</v>
       </c>
       <c r="L94" s="8" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="M94" s="1"/>
       <c r="N94" s="6" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="O94" s="1"/>
       <c r="P94" s="1"/>
@@ -7434,19 +7434,19 @@
         <v>2020</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="G95" s="8" t="s">
         <v>21</v>
@@ -7464,11 +7464,11 @@
         <v>22</v>
       </c>
       <c r="L95" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M95" s="1"/>
       <c r="N95" s="6" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="O95" s="1"/>
       <c r="P95" s="1"/>
@@ -7481,16 +7481,16 @@
         <v>226</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="G96" s="8" t="s">
         <v>21</v>
@@ -7508,11 +7508,11 @@
         <v>22</v>
       </c>
       <c r="L96" s="8" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="M96" s="1"/>
       <c r="N96" s="11" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="O96" s="1"/>
       <c r="P96" s="1"/>
@@ -7522,19 +7522,19 @@
         <v>2021</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="G97" s="8" t="s">
         <v>21</v>
@@ -7552,11 +7552,11 @@
         <v>22</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="M97" s="1"/>
       <c r="N97" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="O97" s="1"/>
       <c r="P97" s="1"/>
@@ -7566,19 +7566,19 @@
         <v>2021</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="G98" s="8" t="s">
         <v>21</v>
@@ -7593,16 +7593,16 @@
         <v>32</v>
       </c>
       <c r="K98" s="1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="L98" s="8" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="M98" s="1" t="s">
         <v>54</v>
       </c>
       <c r="N98" s="9" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="O98" s="1"/>
       <c r="P98" s="1"/>
@@ -7612,19 +7612,19 @@
         <v>2021</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>31</v>
@@ -7639,14 +7639,14 @@
         <v>88</v>
       </c>
       <c r="K99" s="1" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="L99" s="1" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="M99" s="1"/>
       <c r="N99" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="O99" s="1"/>
       <c r="P99" s="1"/>
@@ -7656,19 +7656,19 @@
         <v>2021</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="G100" s="1" t="s">
         <v>31</v>
@@ -7683,16 +7683,16 @@
         <v>88</v>
       </c>
       <c r="K100" s="1" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L100" s="8" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="M100" s="1" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N100" s="6" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="O100" s="1"/>
       <c r="P100" s="1"/>
@@ -7702,19 +7702,19 @@
         <v>2018</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>21</v>
@@ -7729,14 +7729,14 @@
         <v>88</v>
       </c>
       <c r="K101" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L101" s="8" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="M101" s="1"/>
       <c r="N101" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="O101" s="1"/>
       <c r="P101" s="1"/>
@@ -7746,19 +7746,19 @@
         <v>2019</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>21</v>
@@ -7773,14 +7773,14 @@
         <v>88</v>
       </c>
       <c r="K102" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L102" s="8" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="M102" s="1"/>
       <c r="N102" s="6" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="O102" s="1"/>
       <c r="P102" s="1"/>
@@ -7790,19 +7790,19 @@
         <v>2020</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E103" s="8" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="G103" s="8" t="s">
         <v>21</v>
@@ -7817,14 +7817,14 @@
         <v>88</v>
       </c>
       <c r="K103" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L103" s="8" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="M103" s="1"/>
       <c r="N103" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="O103" s="1"/>
       <c r="P103" s="1"/>
@@ -7834,19 +7834,19 @@
         <v>2020</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F104" s="8" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="G104" s="8" t="s">
         <v>21</v>
@@ -7861,14 +7861,14 @@
         <v>88</v>
       </c>
       <c r="K104" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="L104" s="8" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="M104" s="1"/>
       <c r="N104" s="6" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="O104" s="1"/>
       <c r="P104" s="1"/>
@@ -7881,16 +7881,16 @@
         <v>86</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D105" s="8" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F105" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="G105" s="8" t="s">
         <v>21</v>
@@ -7908,11 +7908,11 @@
         <v>89</v>
       </c>
       <c r="L105" s="8" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="M105" s="1"/>
       <c r="N105" s="11" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="O105" s="1"/>
       <c r="P105" s="1"/>
@@ -7922,19 +7922,19 @@
         <v>2021</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C106" s="5" t="s">
         <v>250</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G106" s="5" t="s">
         <v>21</v>
@@ -7952,13 +7952,13 @@
         <v>22</v>
       </c>
       <c r="L106" s="5" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="M106" s="5" t="s">
         <v>54</v>
       </c>
       <c r="N106" s="11" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="107" s="5" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7966,19 +7966,19 @@
         <v>2005</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C107" s="5" t="s">
         <v>250</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E107" s="8" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G107" s="8" t="s">
         <v>21</v>
@@ -7996,11 +7996,11 @@
         <v>22</v>
       </c>
       <c r="L107" s="8" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="M107" s="1"/>
       <c r="N107" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="O107" s="1"/>
       <c r="P107" s="1"/>
@@ -8010,13 +8010,13 @@
         <v>2021</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C108" s="5" t="s">
         <v>250</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>457</v>
+        <v>295</v>
       </c>
       <c r="E108" s="5" t="s">
         <v>458</v>
@@ -8057,13 +8057,13 @@
         <v>250</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G109" s="5" t="s">
         <v>21</v>
@@ -8102,7 +8102,7 @@
       </c>
       <c r="E110" s="1"/>
       <c r="F110" s="8" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G110" s="1" t="s">
         <v>31</v>
@@ -8142,7 +8142,7 @@
         <v>250</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>457</v>
+        <v>295</v>
       </c>
       <c r="E111" s="5" t="s">
         <v>458</v>
@@ -8186,7 +8186,7 @@
         <v>250</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>457</v>
+        <v>295</v>
       </c>
       <c r="E112" s="5" t="s">
         <v>458</v>
@@ -8318,7 +8318,7 @@
         <v>250</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>457</v>
+        <v>295</v>
       </c>
       <c r="E115" s="5" t="s">
         <v>485</v>
@@ -8368,7 +8368,7 @@
         <v>489</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G116" s="5" t="s">
         <v>31</v>
@@ -8412,7 +8412,7 @@
         <v>489</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G117" s="5" t="s">
         <v>31</v>
@@ -8450,13 +8450,13 @@
         <v>250</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>494</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G118" s="1" t="s">
         <v>21</v>
@@ -8496,13 +8496,13 @@
         <v>250</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>457</v>
+        <v>295</v>
       </c>
       <c r="E119" s="5" t="s">
         <v>497</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G119" s="5" t="s">
         <v>22</v>
@@ -8542,13 +8542,13 @@
         <v>250</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E120" s="1" t="s">
         <v>500</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G120" s="1" t="s">
         <v>22</v>
@@ -8632,13 +8632,13 @@
         <v>250</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E122" s="1" t="s">
         <v>505</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>21</v>
@@ -8682,7 +8682,7 @@
         <v>489</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G123" s="5" t="s">
         <v>31</v>
@@ -8761,13 +8761,13 @@
         <v>250</v>
       </c>
       <c r="D125" s="5" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F125" s="8" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G125" s="8" t="s">
         <v>31</v>
@@ -8799,7 +8799,7 @@
         <v>2017</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C126" s="5" t="s">
         <v>250</v>
@@ -8826,7 +8826,7 @@
         <v>88</v>
       </c>
       <c r="K126" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L126" s="5" t="s">
         <v>517</v>
@@ -8843,7 +8843,7 @@
         <v>2019</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>250</v>
@@ -8870,7 +8870,7 @@
         <v>88</v>
       </c>
       <c r="K127" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L127" s="1" t="s">
         <v>519</v>
@@ -8893,13 +8893,13 @@
         <v>250</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E128" s="5" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G128" s="5" t="s">
         <v>21</v>
@@ -8920,7 +8920,7 @@
         <v>522</v>
       </c>
       <c r="M128" s="5" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="N128" s="11" t="s">
         <v>523</v>
@@ -8943,7 +8943,7 @@
         <v>489</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G129" s="5" t="s">
         <v>31</v>
@@ -8964,7 +8964,7 @@
         <v>525</v>
       </c>
       <c r="M129" s="5" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N129" s="7" t="s">
         <v>526</v>
@@ -8987,7 +8987,7 @@
         <v>489</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G130" s="5" t="s">
         <v>21</v>
@@ -9028,7 +9028,7 @@
         <v>489</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G131" s="5" t="s">
         <v>31</v>
@@ -9110,7 +9110,7 @@
         <v>489</v>
       </c>
       <c r="F133" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G133" s="5" t="s">
         <v>31</v>
@@ -9151,7 +9151,7 @@
         <v>489</v>
       </c>
       <c r="F134" s="5" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G134" s="5" t="s">
         <v>21</v>
@@ -9195,7 +9195,7 @@
         <v>489</v>
       </c>
       <c r="F135" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G135" s="5" t="s">
         <v>31</v>
@@ -9239,7 +9239,7 @@
         <v>489</v>
       </c>
       <c r="F136" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G136" s="5" t="s">
         <v>31</v>
@@ -9283,7 +9283,7 @@
         <v>551</v>
       </c>
       <c r="F137" s="8" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G137" s="8" t="s">
         <v>21</v>
@@ -9324,7 +9324,7 @@
         <v>551</v>
       </c>
       <c r="F138" s="8" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G138" s="8" t="s">
         <v>21</v>
@@ -9365,7 +9365,7 @@
         <v>534</v>
       </c>
       <c r="F139" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G139" s="5" t="s">
         <v>31</v>
@@ -9380,7 +9380,7 @@
         <v>32</v>
       </c>
       <c r="K139" s="5" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="L139" s="5" t="s">
         <v>559</v>
@@ -9411,7 +9411,7 @@
         <v>534</v>
       </c>
       <c r="F140" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G140" s="5" t="s">
         <v>21</v>
@@ -9455,7 +9455,7 @@
         <v>534</v>
       </c>
       <c r="F141" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G141" s="5" t="s">
         <v>21</v>
@@ -9499,7 +9499,7 @@
         <v>534</v>
       </c>
       <c r="F142" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G142" s="5" t="s">
         <v>21</v>
@@ -9514,7 +9514,7 @@
         <v>88</v>
       </c>
       <c r="K142" s="5" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L142" s="5" t="s">
         <v>568</v>
@@ -9545,7 +9545,7 @@
         <v>550</v>
       </c>
       <c r="F143" s="8" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G143" s="8" t="s">
         <v>21</v>
@@ -9560,7 +9560,7 @@
         <v>88</v>
       </c>
       <c r="K143" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L143" s="8" t="s">
         <v>571</v>
@@ -9586,7 +9586,7 @@
         <v>534</v>
       </c>
       <c r="F144" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G144" s="5" t="s">
         <v>21</v>
@@ -9632,7 +9632,7 @@
         <v>534</v>
       </c>
       <c r="F145" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G145" s="5" t="s">
         <v>21</v>
@@ -9653,7 +9653,7 @@
         <v>577</v>
       </c>
       <c r="M145" s="5" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N145" s="6" t="s">
         <v>578</v>
@@ -9678,7 +9678,7 @@
         <v>534</v>
       </c>
       <c r="F146" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G146" s="5" t="s">
         <v>21</v>
@@ -9699,7 +9699,7 @@
         <v>580</v>
       </c>
       <c r="M146" s="5" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N146" s="7" t="s">
         <v>581</v>
@@ -9856,7 +9856,7 @@
         <v>534</v>
       </c>
       <c r="F150" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G150" s="5" t="s">
         <v>21</v>
@@ -9900,7 +9900,7 @@
         <v>534</v>
       </c>
       <c r="F151" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G151" s="5" t="s">
         <v>21</v>
@@ -9944,7 +9944,7 @@
         <v>534</v>
       </c>
       <c r="F152" s="5" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G152" s="5" t="s">
         <v>31</v>
@@ -9976,7 +9976,7 @@
         <v>2019</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>603</v>
@@ -10006,7 +10006,7 @@
         <v>605</v>
       </c>
       <c r="M153" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N153" s="2" t="s">
         <v>606</v>
@@ -10047,7 +10047,7 @@
         <v>608</v>
       </c>
       <c r="M154" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N154" s="9" t="s">
         <v>609</v>
@@ -10384,7 +10384,7 @@
         <v>2015</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>603</v>
@@ -10411,7 +10411,7 @@
         <v>22</v>
       </c>
       <c r="L163" s="8" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="N163" s="2" t="s">
         <v>639</v>
@@ -10536,7 +10536,7 @@
         <v>2017</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>603</v>
@@ -10726,7 +10726,7 @@
         <v>2020</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C172" s="8" t="s">
         <v>603</v>
@@ -11014,7 +11014,7 @@
         <v>603</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G179" s="8" t="s">
         <v>21</v>
@@ -11029,7 +11029,7 @@
         <v>32</v>
       </c>
       <c r="K179" s="8" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="L179" s="8" t="s">
         <v>693</v>
@@ -11093,7 +11093,7 @@
         <v>603</v>
       </c>
       <c r="E181" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>700</v>
@@ -12098,13 +12098,13 @@
         <v>88</v>
       </c>
       <c r="K205" s="12" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L205" s="8" t="s">
         <v>769</v>
       </c>
       <c r="M205" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N205" s="2" t="s">
         <v>770</v>
@@ -12115,7 +12115,7 @@
         <v>2017</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>603</v>
@@ -12139,13 +12139,13 @@
         <v>88</v>
       </c>
       <c r="K206" s="12" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L206" s="8" t="s">
         <v>772</v>
       </c>
       <c r="M206" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N206" s="2" t="s">
         <v>773</v>
@@ -12180,13 +12180,13 @@
         <v>88</v>
       </c>
       <c r="K207" s="12" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="L207" s="8" t="s">
         <v>775</v>
       </c>
       <c r="M207" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N207" s="2" t="s">
         <v>776</v>
@@ -12197,7 +12197,7 @@
         <v>2017</v>
       </c>
       <c r="B208" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C208" s="1" t="s">
         <v>603</v>
@@ -12221,13 +12221,13 @@
         <v>88</v>
       </c>
       <c r="K208" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L208" s="8" t="s">
         <v>778</v>
       </c>
       <c r="M208" s="8" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="N208" s="6" t="s">
         <v>779</v>
@@ -12238,7 +12238,7 @@
         <v>2018</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>603</v>
@@ -12262,7 +12262,7 @@
         <v>88</v>
       </c>
       <c r="K209" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L209" s="8" t="s">
         <v>780</v>
@@ -12276,7 +12276,7 @@
         <v>2018</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>603</v>
@@ -12300,7 +12300,7 @@
         <v>88</v>
       </c>
       <c r="K210" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L210" s="8" t="s">
         <v>782</v>
@@ -12314,7 +12314,7 @@
         <v>2018</v>
       </c>
       <c r="B211" s="8" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C211" s="8" t="s">
         <v>603</v>
@@ -12335,7 +12335,7 @@
         <v>88</v>
       </c>
       <c r="K211" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L211" s="8" t="s">
         <v>785</v>
@@ -12373,7 +12373,7 @@
         <v>88</v>
       </c>
       <c r="K212" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L212" s="1" t="s">
         <v>788</v>
@@ -12387,16 +12387,16 @@
         <v>2019</v>
       </c>
       <c r="B213" s="8" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C213" s="8" t="s">
         <v>603</v>
       </c>
       <c r="E213" s="8" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F213" s="1" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="G213" s="8" t="s">
         <v>21</v>
@@ -12411,7 +12411,7 @@
         <v>88</v>
       </c>
       <c r="K213" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L213" s="8" t="s">
         <v>790</v>
@@ -12450,7 +12450,7 @@
         <v>88</v>
       </c>
       <c r="K214" s="1" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="L214" s="8" t="s">
         <v>793</v>
@@ -12577,7 +12577,7 @@
         <v>801</v>
       </c>
       <c r="M217" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N217" s="9" t="s">
         <v>802</v>
@@ -12817,7 +12817,7 @@
         <v>820</v>
       </c>
       <c r="M223" s="8" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="N223" s="2" t="s">
         <v>821</v>
@@ -13103,7 +13103,7 @@
   <dimension ref="A2:F15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="58:58 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="65:65 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13251,7 +13251,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="58:58 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="65:65 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fix paper tested on hardware
</commit_message>
<xml_diff>
--- a/AutonomousRacing_Literature.xlsx
+++ b/AutonomousRacing_Literature.xlsx
@@ -2982,7 +2982,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3171,11 +3171,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="40368462"/>
-        <c:axId val="27764572"/>
+        <c:axId val="50835874"/>
+        <c:axId val="60884291"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="40368462"/>
+        <c:axId val="50835874"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="2009"/>
@@ -3253,13 +3253,13 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27764572"/>
+        <c:crossAx val="60884291"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="27764572"/>
+        <c:axId val="60884291"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3336,7 +3336,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40368462"/>
+        <c:crossAx val="50835874"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3410,8 +3410,10 @@
   </sheetPr>
   <dimension ref="A1:P228"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B49" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F70" activeCellId="0" sqref="F70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A71" activeCellId="0" sqref="71:71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6419,7 +6421,7 @@
         <v>21</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>31</v>
@@ -13103,7 +13105,7 @@
   <dimension ref="A2:F15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="71:71 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13251,7 +13253,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="71:71 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.609375" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>